<commit_message>
updated design metrics. still need some understandability scores.
</commit_message>
<xml_diff>
--- a/documents/Design/SpaceEfficiency.xlsx
+++ b/documents/Design/SpaceEfficiency.xlsx
@@ -38,13 +38,13 @@
     <t>143 bytes of memory</t>
   </si>
   <si>
-    <t>Users.js Modelt</t>
-  </si>
-  <si>
     <t>90 bytes of memory</t>
   </si>
   <si>
     <t>each user takes</t>
+  </si>
+  <si>
+    <t>Users.js Model</t>
   </si>
 </sst>
 </file>
@@ -428,7 +428,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,7 +485,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -493,10 +493,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" s="4"/>
     </row>

</xml_diff>

<commit_message>
wrong issue branch, but space efficiency metric updated in design.
</commit_message>
<xml_diff>
--- a/documents/Design/SpaceEfficiency.xlsx
+++ b/documents/Design/SpaceEfficiency.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>Space Effeciency</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Users.js Model</t>
+  </si>
+  <si>
+    <t>117 bytes of memory</t>
   </si>
 </sst>
 </file>
@@ -428,13 +431,15 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1"/>
+    <col min="5" max="5" width="33" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
@@ -442,15 +447,22 @@
         <v>42682</v>
       </c>
       <c r="C1" s="1"/>
+      <c r="D1" s="1">
+        <v>42704</v>
+      </c>
     </row>
     <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G4" s="4"/>
@@ -460,6 +472,9 @@
         <v>1</v>
       </c>
       <c r="C5" s="4"/>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -470,17 +485,26 @@
         <v>3</v>
       </c>
       <c r="C6" s="4"/>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
+      <c r="E7" s="4"/>
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -489,6 +513,10 @@
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
+      <c r="D9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="4"/>
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -499,6 +527,12 @@
         <v>4</v>
       </c>
       <c r="C10" s="4"/>
+      <c r="D10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C11" s="1"/>

</xml_diff>

<commit_message>
created graphs. fixed testability metric.
</commit_message>
<xml_diff>
--- a/documents/Design/SpaceEfficiency.xlsx
+++ b/documents/Design/SpaceEfficiency.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>Space Effeciency</t>
   </si>
@@ -49,11 +49,23 @@
   <si>
     <t>117 bytes of memory</t>
   </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Posts Model</t>
+  </si>
+  <si>
+    <t>Users Model</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm;@"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -105,7 +117,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -114,6 +126,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -129,6 +145,1162 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Space Efficiency: Byte</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>s Used by Models</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SpaceEfficiency!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Posts Model</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>SpaceEfficiency!$F$3:$F$4</c:f>
+              <c:numCache>
+                <c:formatCode>[$-409]d\-mmm;@</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>42682</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42704</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>SpaceEfficiency!$G$3:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>143</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9749-4F05-92CB-42FA0A538BA0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>SpaceEfficiency!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Users Model</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>SpaceEfficiency!$F$3:$F$4</c:f>
+              <c:numCache>
+                <c:formatCode>[$-409]d\-mmm;@</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>42682</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42704</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>SpaceEfficiency!$H$3:$H$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>117</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9749-4F05-92CB-42FA0A538BA0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="369505352"/>
+        <c:axId val="369509288"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="369505352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="[$-409]d\-mmm;@" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="369509288"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="369509288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t># of Bytes per Document</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="369505352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1904999</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>147636</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AAF2F08-D1E9-4159-8819-B2EE29F282ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -428,10 +1600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,9 +1612,12 @@
     <col min="2" max="2" width="28.85546875" customWidth="1"/>
     <col min="4" max="4" width="25.28515625" customWidth="1"/>
     <col min="5" max="5" width="33" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="1">
         <v>42682</v>
       </c>
@@ -451,11 +1626,20 @@
         <v>42704</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -463,11 +1647,28 @@
       <c r="D3" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F3" s="6">
+        <v>42682</v>
+      </c>
+      <c r="G3">
+        <v>143</v>
+      </c>
+      <c r="H3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="F4" s="6">
+        <v>42704</v>
+      </c>
+      <c r="G4" s="7">
+        <v>143</v>
+      </c>
+      <c r="H4">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -477,7 +1678,7 @@
       </c>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -493,13 +1694,13 @@
       </c>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="E7" s="4"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -507,7 +1708,7 @@
       <c r="E8" s="4"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -519,7 +1720,7 @@
       <c r="E9" s="4"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
@@ -534,24 +1735,24 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="D12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -559,7 +1760,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -589,5 +1790,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>